<commit_message>
edit in Main Data Collection
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="10">
   <si>
     <t>Actions</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1">
         <v>43429</v>
@@ -423,7 +426,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>43029</v>
@@ -440,7 +443,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1">
         <v>43175</v>
@@ -457,7 +460,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1">
         <v>43064</v>
@@ -474,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1">
         <v>42917</v>
@@ -491,7 +494,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1">
         <v>43013</v>
@@ -508,7 +511,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1">
         <v>42927</v>
@@ -525,7 +528,7 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1">
         <v>43365</v>
@@ -542,7 +545,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1">
         <v>43467</v>
@@ -559,7 +562,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1">
         <v>43197</v>
@@ -593,7 +596,7 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F13" s="1">
         <v>43467</v>
@@ -610,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1">
         <v>42737</v>

</xml_diff>

<commit_message>
Bug Fix - Retrieve single item
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -400,7 +400,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>758704</v>
+        <v>809944</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -409,15 +409,15 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1">
-        <v>43429</v>
+        <v>43232</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>894544</v>
+        <v>619534</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -426,15 +426,15 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1">
-        <v>43029</v>
+        <v>43143</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>446814</v>
+        <v>532044</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -443,15 +443,15 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1">
-        <v>43175</v>
+        <v>42903</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>766604</v>
+        <v>612294</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -460,15 +460,15 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1">
-        <v>43064</v>
+        <v>42895</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>535144</v>
+        <v>640094</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -477,15 +477,15 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1">
-        <v>42917</v>
+        <v>42996</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>604714</v>
+        <v>655994</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -494,15 +494,15 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1">
-        <v>43013</v>
+        <v>43171</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>904844</v>
+        <v>640314</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -511,15 +511,15 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1">
-        <v>42927</v>
+        <v>43294</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>189244</v>
+        <v>637964</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -528,15 +528,15 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="1">
-        <v>43365</v>
+        <v>43227</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>827104</v>
+        <v>193134</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -545,15 +545,15 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1">
-        <v>43467</v>
+        <v>43193</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>514884</v>
+        <v>798064</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -562,15 +562,15 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1">
-        <v>43197</v>
+        <v>42913</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>328104</v>
+        <v>442854</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -582,12 +582,12 @@
         <v>8</v>
       </c>
       <c r="F12" s="1">
-        <v>43396</v>
+        <v>42995</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>456974</v>
+        <v>563864</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -596,10 +596,10 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1">
-        <v>43467</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>